<commit_message>
EPF modification for part E
</commit_message>
<xml_diff>
--- a/开发文档/整体方案/HR Localization_Oversea_V3.0.xlsx
+++ b/开发文档/整体方案/HR Localization_Oversea_V3.0.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\project\HR本地化\马来本地化\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Devlop\eclipse\workspace\HRLocalization\开发文档\整体方案\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="8140" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="8145" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="名词解释" sheetId="7" r:id="rId1"/>
@@ -1901,9 +1901,6 @@
     <t>Is Voluntary EPF</t>
   </si>
   <si>
-    <t>hrlocal-000033</t>
-  </si>
-  <si>
     <t>hrlocal-000034</t>
   </si>
   <si>
@@ -1920,6 +1917,9 @@
   </si>
   <si>
     <t>31/12/2018 变更 支持雇员自由选择比率缴纳EPF</t>
+  </si>
+  <si>
+    <t>hrlocal-000035</t>
   </si>
 </sst>
 </file>
@@ -2215,6 +2215,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2224,8 +2226,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2634,14 +2634,14 @@
       <selection activeCell="B14" sqref="B14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.7109375" style="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" ht="15">
       <c r="B4" s="19" t="s">
         <v>167</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" ht="15">
       <c r="B6" s="19" t="s">
         <v>169</v>
       </c>
@@ -2676,24 +2676,24 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" ht="16.5">
       <c r="B12" s="17" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" ht="16.5">
       <c r="B13" s="18" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="14" spans="2:6" ht="165.65" customHeight="1">
-      <c r="B14" s="35" t="s">
+    <row r="14" spans="2:6" ht="165.6" customHeight="1">
+      <c r="B14" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2711,7 +2711,7 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2726,7 +2726,7 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -2749,7 +2749,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5">
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="14" t="s">
         <v>280</v>
       </c>
@@ -2771,9 +2771,9 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3">
@@ -2817,19 +2817,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43:G44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.26953125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="33.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3045,7 +3045,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="56">
+    <row r="17" spans="1:8" ht="57">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="42">
+    <row r="18" spans="1:8" ht="42.75">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="28.5">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="28">
+    <row r="36" spans="1:8" ht="28.5">
       <c r="A36" s="4" t="s">
         <v>4</v>
       </c>
@@ -3580,7 +3580,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="28" customHeight="1">
+    <row r="43" spans="1:8" ht="27.95" customHeight="1">
       <c r="A43" s="4" t="s">
         <v>4</v>
       </c>
@@ -3597,8 +3597,8 @@
         <v>524</v>
       </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="36" t="s">
-        <v>526</v>
+      <c r="G43" s="38" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="16.5" customHeight="1">
@@ -3615,10 +3615,10 @@
         <v>238</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="F44" s="4"/>
-      <c r="G44" s="37"/>
+      <c r="G44" s="39"/>
     </row>
     <row r="45" spans="1:8" ht="16.5" customHeight="1">
       <c r="A45" s="4"/>
@@ -3701,13 +3701,13 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1796875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3720,7 +3720,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
@@ -3873,14 +3873,14 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="12.54296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="2" width="8.7109375" style="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="3:7" ht="18" customHeight="1">
@@ -3897,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="3:7">
+    <row r="8" spans="3:7" ht="28.5">
       <c r="C8" s="4"/>
       <c r="D8" s="6" t="s">
         <v>180</v>
@@ -3985,14 +3985,14 @@
       <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.81640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.6328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="41.6328125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4020,7 +4020,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="28" customFormat="1" ht="56">
+    <row r="8" spans="1:8" s="28" customFormat="1" ht="57">
       <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28">
+    <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28">
+    <row r="10" spans="1:8" ht="28.5">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" ht="15">
       <c r="A23" s="2" t="s">
         <v>71</v>
       </c>
@@ -4260,7 +4260,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" s="28" customFormat="1" ht="56">
+    <row r="25" spans="1:5" s="28" customFormat="1" ht="57">
       <c r="A25" s="26"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26" t="s">
@@ -4271,7 +4271,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="28" customFormat="1" ht="56">
+    <row r="26" spans="1:5" s="28" customFormat="1" ht="57">
       <c r="A26" s="26"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29" t="s">
@@ -4441,7 +4441,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" ht="28">
+    <row r="40" spans="1:5" ht="28.5">
       <c r="A40" s="4" t="s">
         <v>389</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="28">
+    <row r="41" spans="1:5" ht="28.5">
       <c r="A41" s="4" t="s">
         <v>390</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28">
+    <row r="42" spans="1:5" ht="28.5">
       <c r="A42" s="4" t="s">
         <v>391</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="28">
+    <row r="45" spans="1:5" ht="28.5">
       <c r="A45" s="4" t="s">
         <v>487</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="28">
+    <row r="46" spans="1:5" ht="28.5">
       <c r="A46" s="4" t="s">
         <v>488</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="42">
+    <row r="47" spans="1:5" ht="42.75">
       <c r="A47" s="4" t="s">
         <v>489</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="42">
+    <row r="48" spans="1:5" ht="57">
       <c r="A48" s="4" t="s">
         <v>490</v>
       </c>
@@ -4837,13 +4837,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -4881,7 +4881,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="B9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K9" t="s">
         <v>139</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="B10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="K10" t="s">
         <v>131</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="B11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K11" t="s">
         <v>132</v>
@@ -5098,61 +5098,61 @@
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="38" t="s">
-        <v>530</v>
-      </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
+      <c r="B42" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
       <c r="K42" s="13" t="s">
         <v>466</v>
       </c>
       <c r="L42" s="13"/>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="39" t="s">
-        <v>527</v>
-      </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
+      <c r="B43" s="36" t="s">
+        <v>526</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
       <c r="K43" s="13"/>
       <c r="L43" s="13" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="36" t="s">
+        <v>527</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="L44" s="13"/>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="B45" s="36" t="s">
         <v>528</v>
       </c>
-      <c r="C44" s="39"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="L44" s="13"/>
-    </row>
-    <row r="45" spans="2:12">
-      <c r="B45" s="39" t="s">
-        <v>529</v>
-      </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
       <c r="K45" t="s">
         <v>200</v>
       </c>
@@ -5539,12 +5539,12 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -5572,7 +5572,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.5">
+    <row r="8" spans="1:13" ht="15.75">
       <c r="A8" s="14" t="s">
         <v>262</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60">
+    <row r="9" spans="1:13" ht="63">
       <c r="A9" s="15" t="s">
         <v>146</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15">
+    <row r="10" spans="1:13" ht="15.75">
       <c r="A10" s="15" t="s">
         <v>151</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15">
+    <row r="11" spans="1:13" ht="15.75">
       <c r="A11" s="15" t="s">
         <v>154</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15">
+    <row r="12" spans="1:13" ht="15.75">
       <c r="A12" s="15" t="s">
         <v>157</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13" ht="15.75">
       <c r="A13" s="15" t="s">
         <v>158</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15">
+    <row r="14" spans="1:13" ht="15.75">
       <c r="A14" s="15" t="s">
         <v>159</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15">
+    <row r="15" spans="1:13" ht="15.75">
       <c r="A15" s="15" t="s">
         <v>160</v>
       </c>
@@ -5705,7 +5705,7 @@
         <v>10900</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13" ht="15.75">
       <c r="A16" s="15" t="s">
         <v>161</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>46900</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="15" t="s">
         <v>162</v>
       </c>
@@ -5739,7 +5739,7 @@
         <v>83650</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15">
+    <row r="18" spans="1:5" ht="31.5">
       <c r="A18" s="15" t="s">
         <v>163</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>133650</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30">
+    <row r="19" spans="1:5" ht="31.5">
       <c r="A19" s="15" t="s">
         <v>164</v>
       </c>
@@ -5786,12 +5786,12 @@
       <selection activeCell="B28" sqref="B28:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="37.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.54296875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5816,7 +5816,7 @@
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="20.5" customHeight="1">
+    <row r="6" spans="1:6" ht="20.45" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>76</v>
       </c>

</xml_diff>